<commit_message>
add delete memo ujroh
</commit_message>
<xml_diff>
--- a/public/migrasi/migrasi-np.xlsx
+++ b/public/migrasi/migrasi-np.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramdoni/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FC231-6864-864D-AFB2-C6FCB4A99AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F889CBF-1BBC-F649-A3F6-2262D9EC490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{6ED93D9F-06CA-0A46-B5DD-9329E59AB019}"/>
+    <workbookView xWindow="-25600" yWindow="1220" windowWidth="25600" windowHeight="18520" xr2:uid="{6ED93D9F-06CA-0A46-B5DD-9329E59AB019}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -502,7 +512,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +524,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -539,9 +560,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,14 +883,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E185C091-32A0-7A41-9EAB-FE72710C115A}">
   <dimension ref="A1:AB85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="58.6640625" customWidth="1"/>
-    <col min="5" max="10" width="10.83203125" style="1"/>
+    <col min="5" max="10" width="10.83203125" style="4"/>
     <col min="11" max="11" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="54.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="27.5" bestFit="1" customWidth="1"/>
@@ -874,89 +898,89 @@
     <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -973,22 +997,22 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
         <v>0.1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="4">
         <v>0.2</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
         <v>0</v>
       </c>
       <c r="K2" t="s">
@@ -1059,22 +1083,22 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.15</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>0.2</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
         <v>0</v>
       </c>
       <c r="K3" t="s">
@@ -1145,22 +1169,22 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
@@ -1231,22 +1255,22 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>0.15</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>0.2</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
         <v>0</v>
       </c>
       <c r="K5" t="s">
@@ -1317,22 +1341,22 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>0.27500000000000002</v>
       </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
         <v>0</v>
       </c>
       <c r="K6" t="s">
@@ -1403,22 +1427,22 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>0.1</v>
       </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
         <v>0</v>
       </c>
       <c r="K7" t="s">
@@ -1489,22 +1513,22 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
         <v>0.125</v>
       </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1575,22 +1599,22 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
         <v>0</v>
       </c>
       <c r="K9" t="s">
@@ -1661,22 +1685,22 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>0.115</v>
       </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
         <v>0</v>
       </c>
       <c r="K10" t="s">
@@ -1747,22 +1771,22 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>0.125</v>
       </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
         <v>0</v>
       </c>
       <c r="K11" t="s">
@@ -1833,22 +1857,22 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
         <v>0.25</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>0.05</v>
       </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
         <v>0</v>
       </c>
       <c r="K12" t="s">
@@ -1919,22 +1943,22 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
         <v>0.1326</v>
       </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
         <v>0</v>
       </c>
       <c r="K13" t="s">
@@ -2005,22 +2029,22 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
         <v>0.1326</v>
       </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
         <v>0</v>
       </c>
       <c r="K14" t="s">
@@ -2091,22 +2115,22 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
         <v>0.25</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <v>0.05</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
         <v>0</v>
       </c>
       <c r="K15" t="s">
@@ -2177,22 +2201,22 @@
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
         <v>0</v>
       </c>
       <c r="K16" t="s">
@@ -2263,22 +2287,22 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
         <v>0</v>
       </c>
       <c r="K17" t="s">
@@ -2349,22 +2373,22 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
         <v>0.2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>0.1</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
         <v>0</v>
       </c>
       <c r="K18" t="s">
@@ -2435,22 +2459,22 @@
       <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
         <v>0.02</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
         <v>0</v>
       </c>
       <c r="K19" t="s">
@@ -2521,22 +2545,22 @@
       <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
         <v>0.01</v>
       </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
         <v>0</v>
       </c>
       <c r="K20" t="s">
@@ -2607,22 +2631,22 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
         <v>0.2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="4">
         <v>0.1</v>
       </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
         <v>0</v>
       </c>
       <c r="K21" t="s">
@@ -2693,22 +2717,22 @@
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
         <v>0.2</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="4">
         <v>0.1</v>
       </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1">
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
         <v>0</v>
       </c>
       <c r="K22" t="s">
@@ -2779,22 +2803,22 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
         <v>0.27500000000000002</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
         <v>0</v>
       </c>
       <c r="K23" t="s">
@@ -2865,22 +2889,22 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
         <v>0.2</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
         <v>0.1</v>
       </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
         <v>0</v>
       </c>
       <c r="K24" t="s">
@@ -2903,22 +2927,22 @@
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <v>0.1</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <v>0.2</v>
       </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
         <v>0</v>
       </c>
       <c r="K25" t="s">
@@ -2989,22 +3013,22 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
         <v>0.05</v>
       </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
         <v>0</v>
       </c>
       <c r="K26" t="s">
@@ -3075,22 +3099,22 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
         <v>0.22500000000000001</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="4">
         <v>0.05</v>
       </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
         <v>0</v>
       </c>
       <c r="K27" t="s">
@@ -3152,22 +3176,22 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
         <v>0.2</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="4">
         <v>0.1</v>
       </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4">
         <v>0</v>
       </c>
       <c r="K28" t="s">
@@ -3238,22 +3262,22 @@
       <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
         <v>0.2</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="4">
         <v>0.1</v>
       </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
         <v>0</v>
       </c>
       <c r="K29" t="s">
@@ -3324,22 +3348,22 @@
       <c r="D30" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
         <v>0.2</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="4">
         <v>0.1</v>
       </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
         <v>0</v>
       </c>
       <c r="K30" t="s">
@@ -3410,22 +3434,22 @@
       <c r="D31" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
         <v>0.2</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="4">
         <v>0.1</v>
       </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
         <v>0</v>
       </c>
       <c r="K31" t="s">
@@ -3496,22 +3520,22 @@
       <c r="D32" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
         <v>0.25</v>
       </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
-      <c r="J32" s="1">
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
         <v>0</v>
       </c>
       <c r="K32" t="s">
@@ -3582,22 +3606,22 @@
       <c r="D33" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
         <v>0.17499999999999999</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4">
         <v>0</v>
       </c>
       <c r="K33" t="s">
@@ -3668,22 +3692,22 @@
       <c r="D34" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="4">
         <v>0.01</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="4">
         <v>0.1</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="4">
         <v>0.15</v>
       </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-      <c r="J34" s="1">
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4">
         <v>0.04</v>
       </c>
       <c r="K34" t="s">
@@ -3754,22 +3778,22 @@
       <c r="D35" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="4">
         <v>0.05</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="4">
         <v>0.25</v>
       </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0</v>
+      </c>
+      <c r="J35" s="4">
         <v>0</v>
       </c>
       <c r="K35" t="s">
@@ -3840,22 +3864,22 @@
       <c r="D36" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="4">
         <v>0.1</v>
       </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4">
         <v>0.25</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="4">
         <v>0</v>
       </c>
       <c r="K36" t="s">
@@ -3926,22 +3950,22 @@
       <c r="D37" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
         <v>0.1</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
-      <c r="J37" s="1">
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4">
         <v>0</v>
       </c>
       <c r="K37" t="s">
@@ -4006,22 +4030,22 @@
       <c r="D38" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="4">
         <v>0.25</v>
       </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
-      <c r="J38" s="1">
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4">
         <v>0</v>
       </c>
       <c r="K38" t="s">
@@ -4092,22 +4116,22 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="4">
         <v>0.25</v>
       </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1">
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I39" s="1">
-        <v>0</v>
-      </c>
-      <c r="J39" s="1">
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4">
         <v>0</v>
       </c>
       <c r="K39" t="s">
@@ -4178,22 +4202,22 @@
       <c r="D40" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1">
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
         <v>0.35</v>
       </c>
-      <c r="H40" s="1">
-        <v>0</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0</v>
-      </c>
-      <c r="J40" s="1">
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4">
         <v>0</v>
       </c>
       <c r="K40" t="s">
@@ -4264,22 +4288,22 @@
       <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="4">
         <v>0.25</v>
       </c>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0</v>
-      </c>
-      <c r="I41" s="1">
-        <v>0</v>
-      </c>
-      <c r="J41" s="1">
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
         <v>0</v>
       </c>
       <c r="K41" t="s">
@@ -4350,22 +4374,22 @@
       <c r="D42" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="4">
         <v>0.1</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="4">
         <v>0.125</v>
       </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0</v>
-      </c>
-      <c r="J42" s="1">
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4">
         <v>0</v>
       </c>
       <c r="K42" t="s">
@@ -4436,22 +4460,22 @@
       <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="4">
         <v>0.15</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="4">
         <v>0.1</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I43" s="1">
-        <v>0</v>
-      </c>
-      <c r="J43" s="1">
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
         <v>0</v>
       </c>
       <c r="K43" t="s">
@@ -4522,22 +4546,22 @@
       <c r="D44" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="4">
         <v>0.05</v>
       </c>
-      <c r="F44" s="1">
-        <v>0</v>
-      </c>
-      <c r="G44" s="1">
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
         <v>0.3</v>
       </c>
-      <c r="H44" s="1">
-        <v>0</v>
-      </c>
-      <c r="I44" s="1">
-        <v>0</v>
-      </c>
-      <c r="J44" s="1">
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
         <v>0</v>
       </c>
       <c r="K44" t="s">
@@ -4608,22 +4632,22 @@
       <c r="D45" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1">
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H45" s="1">
-        <v>0</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0</v>
-      </c>
-      <c r="J45" s="1">
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
         <v>0</v>
       </c>
       <c r="K45" t="s">
@@ -4691,22 +4715,22 @@
       <c r="D46" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F46" s="1">
-        <v>0</v>
-      </c>
-      <c r="G46" s="1">
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H46" s="1">
-        <v>0</v>
-      </c>
-      <c r="I46" s="1">
-        <v>0</v>
-      </c>
-      <c r="J46" s="1">
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
         <v>0</v>
       </c>
       <c r="K46" t="s">
@@ -4774,22 +4798,22 @@
       <c r="D47" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F47" s="1">
-        <v>0</v>
-      </c>
-      <c r="G47" s="1">
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H47" s="1">
-        <v>0</v>
-      </c>
-      <c r="I47" s="1">
-        <v>0</v>
-      </c>
-      <c r="J47" s="1">
+      <c r="H47" s="4">
+        <v>0</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
         <v>0</v>
       </c>
       <c r="K47" t="s">
@@ -4857,22 +4881,22 @@
       <c r="D48" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
+      <c r="E48" s="4">
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1">
+      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
         <v>0.05</v>
       </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
-      <c r="J48" s="1">
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
         <v>0</v>
       </c>
       <c r="K48" t="s">
@@ -4940,22 +4964,22 @@
       <c r="D49" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-      <c r="F49" s="1">
+      <c r="E49" s="4">
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="4">
         <v>0.03</v>
       </c>
-      <c r="H49" s="1">
-        <v>0</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="J49" s="1">
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
         <v>0</v>
       </c>
       <c r="K49" t="s">
@@ -5026,22 +5050,22 @@
       <c r="D50" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="4">
         <v>0.1</v>
       </c>
-      <c r="F50" s="1">
-        <v>0</v>
-      </c>
-      <c r="G50" s="1">
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I50" s="1">
-        <v>0</v>
-      </c>
-      <c r="J50" s="1">
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
         <v>0.15</v>
       </c>
       <c r="K50" t="s">
@@ -5112,22 +5136,22 @@
       <c r="D51" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="4">
         <v>0.25</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-      <c r="I51" s="1">
-        <v>0</v>
-      </c>
-      <c r="J51" s="1">
+      <c r="H51" s="4">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
         <v>0</v>
       </c>
       <c r="K51" t="s">
@@ -5198,22 +5222,22 @@
       <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1">
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="F52" s="4">
         <v>0.15</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="4">
         <v>0.2</v>
       </c>
-      <c r="H52" s="1">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1">
-        <v>0</v>
-      </c>
-      <c r="J52" s="1">
+      <c r="H52" s="4">
+        <v>0</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0</v>
+      </c>
+      <c r="J52" s="4">
         <v>0</v>
       </c>
       <c r="K52" t="s">
@@ -5284,22 +5308,22 @@
       <c r="D53" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="4">
         <v>0.01</v>
       </c>
-      <c r="F53" s="1">
-        <v>0</v>
-      </c>
-      <c r="G53" s="1">
+      <c r="F53" s="4">
+        <v>0</v>
+      </c>
+      <c r="G53" s="4">
         <v>0.1</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53" s="4">
         <v>0.06</v>
       </c>
-      <c r="I53" s="1">
-        <v>0</v>
-      </c>
-      <c r="J53" s="1">
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
         <v>0</v>
       </c>
       <c r="K53" t="s">
@@ -5370,22 +5394,22 @@
       <c r="D54" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F54" s="1">
-        <v>0</v>
-      </c>
-      <c r="G54" s="1">
+      <c r="F54" s="4">
+        <v>0</v>
+      </c>
+      <c r="G54" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H54" s="1">
-        <v>0</v>
-      </c>
-      <c r="I54" s="1">
-        <v>0</v>
-      </c>
-      <c r="J54" s="1">
+      <c r="H54" s="4">
+        <v>0</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4">
         <v>0</v>
       </c>
       <c r="K54" t="s">
@@ -5456,22 +5480,22 @@
       <c r="D55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="1">
+      <c r="E55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
         <v>0.3</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="4">
         <v>0.05</v>
       </c>
-      <c r="H55" s="1">
-        <v>0</v>
-      </c>
-      <c r="I55" s="1">
-        <v>0</v>
-      </c>
-      <c r="J55" s="1">
+      <c r="H55" s="4">
+        <v>0</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
         <v>0</v>
       </c>
       <c r="K55" t="s">
@@ -5542,22 +5566,22 @@
       <c r="D56" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="E56" s="4">
+        <v>0</v>
+      </c>
+      <c r="F56" s="4">
         <v>0.15</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G56" s="4">
         <v>0.2</v>
       </c>
-      <c r="H56" s="1">
-        <v>0</v>
-      </c>
-      <c r="I56" s="1">
-        <v>0</v>
-      </c>
-      <c r="J56" s="1">
+      <c r="H56" s="4">
+        <v>0</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
         <v>0</v>
       </c>
       <c r="K56" t="s">
@@ -5628,22 +5652,22 @@
       <c r="D57" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="1">
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
+      <c r="F57" s="4">
         <v>0.15</v>
       </c>
-      <c r="G57" s="1">
+      <c r="G57" s="4">
         <v>0.2</v>
       </c>
-      <c r="H57" s="1">
-        <v>0</v>
-      </c>
-      <c r="I57" s="1">
-        <v>0</v>
-      </c>
-      <c r="J57" s="1">
+      <c r="H57" s="4">
+        <v>0</v>
+      </c>
+      <c r="I57" s="4">
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
         <v>0</v>
       </c>
       <c r="K57" t="s">
@@ -5714,22 +5738,22 @@
       <c r="D58" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F58" s="1">
-        <v>0</v>
-      </c>
-      <c r="G58" s="1">
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="4">
         <v>0.3</v>
       </c>
-      <c r="H58" s="1">
-        <v>0</v>
-      </c>
-      <c r="I58" s="1">
-        <v>0</v>
-      </c>
-      <c r="J58" s="1">
+      <c r="H58" s="4">
+        <v>0</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
         <v>0</v>
       </c>
       <c r="K58" t="s">
@@ -5800,22 +5824,22 @@
       <c r="D59" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="4">
         <v>0.05</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="4">
         <v>0.1</v>
       </c>
-      <c r="G59" s="1">
-        <v>0</v>
-      </c>
-      <c r="H59" s="1">
-        <v>0</v>
-      </c>
-      <c r="I59" s="1">
+      <c r="G59" s="4">
+        <v>0</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0</v>
+      </c>
+      <c r="I59" s="4">
         <v>0.15</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J59" s="4">
         <v>0</v>
       </c>
       <c r="K59" t="s">
@@ -5886,22 +5910,22 @@
       <c r="D60" t="s">
         <v>12</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="4">
         <v>0.25</v>
       </c>
-      <c r="G60" s="1">
+      <c r="G60" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H60" s="1">
-        <v>0</v>
-      </c>
-      <c r="I60" s="1">
-        <v>0</v>
-      </c>
-      <c r="J60" s="1">
+      <c r="H60" s="4">
+        <v>0</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
         <v>0</v>
       </c>
       <c r="K60" t="s">
@@ -5972,22 +5996,22 @@
       <c r="D61" t="s">
         <v>12</v>
       </c>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
-      <c r="F61" s="1">
+      <c r="E61" s="4">
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
         <v>0.125</v>
       </c>
-      <c r="G61" s="1">
-        <v>0</v>
-      </c>
-      <c r="H61" s="1">
+      <c r="G61" s="4">
+        <v>0</v>
+      </c>
+      <c r="H61" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I61" s="1">
-        <v>0</v>
-      </c>
-      <c r="J61" s="1">
+      <c r="I61" s="4">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
         <v>0</v>
       </c>
       <c r="K61" t="s">
@@ -6058,22 +6082,22 @@
       <c r="D62" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="4">
         <v>0.02</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="4">
         <v>0.2</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="4">
         <v>0.01</v>
       </c>
-      <c r="H62" s="1">
-        <v>0</v>
-      </c>
-      <c r="I62" s="1">
-        <v>0</v>
-      </c>
-      <c r="J62" s="1">
+      <c r="H62" s="4">
+        <v>0</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
         <v>0</v>
       </c>
       <c r="K62" t="s">
@@ -6141,22 +6165,22 @@
       <c r="D63" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="1">
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
+      <c r="F63" s="4">
         <v>0.25</v>
       </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1">
+      <c r="G63" s="4">
+        <v>0</v>
+      </c>
+      <c r="H63" s="4">
         <v>0.05</v>
       </c>
-      <c r="I63" s="1">
-        <v>0</v>
-      </c>
-      <c r="J63" s="1">
+      <c r="I63" s="4">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4">
         <v>0</v>
       </c>
       <c r="K63" t="s">
@@ -6227,22 +6251,22 @@
       <c r="D64" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1">
+      <c r="F64" s="4">
+        <v>0</v>
+      </c>
+      <c r="G64" s="4">
         <v>0.125</v>
       </c>
-      <c r="H64" s="1">
-        <v>0</v>
-      </c>
-      <c r="I64" s="1">
-        <v>0</v>
-      </c>
-      <c r="J64" s="1">
+      <c r="H64" s="4">
+        <v>0</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
         <v>0</v>
       </c>
       <c r="K64" t="s">
@@ -6313,22 +6337,22 @@
       <c r="D65" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="4">
         <v>0.15</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="4">
         <v>0.05</v>
       </c>
-      <c r="H65" s="1">
-        <v>0</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
-      <c r="J65" s="1">
+      <c r="H65" s="4">
+        <v>0</v>
+      </c>
+      <c r="I65" s="4">
+        <v>0</v>
+      </c>
+      <c r="J65" s="4">
         <v>0</v>
       </c>
       <c r="K65" t="s">
@@ -6399,22 +6423,22 @@
       <c r="D66" t="s">
         <v>12</v>
       </c>
-      <c r="E66" s="1">
-        <v>0</v>
-      </c>
-      <c r="F66" s="1">
+      <c r="E66" s="4">
+        <v>0</v>
+      </c>
+      <c r="F66" s="4">
         <v>0.05</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="4">
         <v>0.3</v>
       </c>
-      <c r="H66" s="1">
-        <v>0</v>
-      </c>
-      <c r="I66" s="1">
-        <v>0</v>
-      </c>
-      <c r="J66" s="1">
+      <c r="H66" s="4">
+        <v>0</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
         <v>0</v>
       </c>
       <c r="K66" t="s">
@@ -6485,22 +6509,22 @@
       <c r="D67" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="1">
-        <v>0</v>
-      </c>
-      <c r="F67" s="1">
+      <c r="E67" s="4">
+        <v>0</v>
+      </c>
+      <c r="F67" s="4">
         <v>0.05</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G67" s="4">
         <v>0.3</v>
       </c>
-      <c r="H67" s="1">
-        <v>0</v>
-      </c>
-      <c r="I67" s="1">
-        <v>0</v>
-      </c>
-      <c r="J67" s="1">
+      <c r="H67" s="4">
+        <v>0</v>
+      </c>
+      <c r="I67" s="4">
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
         <v>0</v>
       </c>
       <c r="K67" t="s">
@@ -6571,22 +6595,22 @@
       <c r="D68" t="s">
         <v>12</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68" s="4">
         <v>0.25</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G68" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H68" s="1">
-        <v>0</v>
-      </c>
-      <c r="I68" s="1">
-        <v>0</v>
-      </c>
-      <c r="J68" s="1">
+      <c r="H68" s="4">
+        <v>0</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
         <v>0</v>
       </c>
       <c r="K68" t="s">
@@ -6657,22 +6681,22 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="1">
-        <v>0</v>
-      </c>
-      <c r="F69" s="1">
+      <c r="E69" s="4">
+        <v>0</v>
+      </c>
+      <c r="F69" s="4">
         <v>0.05</v>
       </c>
-      <c r="G69" s="1">
+      <c r="G69" s="4">
         <v>0.3</v>
       </c>
-      <c r="H69" s="1">
-        <v>0</v>
-      </c>
-      <c r="I69" s="1">
-        <v>0</v>
-      </c>
-      <c r="J69" s="1">
+      <c r="H69" s="4">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
+      <c r="J69" s="4">
         <v>0</v>
       </c>
       <c r="K69" t="s">
@@ -6743,22 +6767,22 @@
       <c r="D70" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="4">
         <v>0.15</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G70" s="4">
         <v>0.04</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H70" s="4">
         <v>0.01</v>
       </c>
-      <c r="I70" s="1">
-        <v>0</v>
-      </c>
-      <c r="J70" s="1">
+      <c r="I70" s="4">
+        <v>0</v>
+      </c>
+      <c r="J70" s="4">
         <v>0</v>
       </c>
       <c r="K70" t="s">
@@ -6829,22 +6853,22 @@
       <c r="D71" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="1">
-        <v>0</v>
-      </c>
-      <c r="F71" s="1">
-        <v>0</v>
-      </c>
-      <c r="G71" s="1">
-        <v>0</v>
-      </c>
-      <c r="H71" s="1">
+      <c r="E71" s="4">
+        <v>0</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0</v>
+      </c>
+      <c r="H71" s="4">
         <v>0.2</v>
       </c>
-      <c r="I71" s="1">
-        <v>0</v>
-      </c>
-      <c r="J71" s="1">
+      <c r="I71" s="4">
+        <v>0</v>
+      </c>
+      <c r="J71" s="4">
         <v>0</v>
       </c>
       <c r="K71" t="s">
@@ -6915,22 +6939,22 @@
       <c r="D72" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72" s="4">
         <v>0.245</v>
       </c>
-      <c r="G72" s="1">
+      <c r="G72" s="4">
         <v>0.01</v>
       </c>
-      <c r="H72" s="1">
-        <v>0</v>
-      </c>
-      <c r="I72" s="1">
-        <v>0</v>
-      </c>
-      <c r="J72" s="1">
+      <c r="H72" s="4">
+        <v>0</v>
+      </c>
+      <c r="I72" s="4">
+        <v>0</v>
+      </c>
+      <c r="J72" s="4">
         <v>0</v>
       </c>
       <c r="K72" t="s">
@@ -6995,22 +7019,22 @@
       <c r="D73" t="s">
         <v>12</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="4">
         <v>0.05</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="4">
         <v>0.1</v>
       </c>
-      <c r="G73" s="1">
+      <c r="G73" s="4">
         <v>0.15</v>
       </c>
-      <c r="H73" s="1">
-        <v>0</v>
-      </c>
-      <c r="I73" s="1">
-        <v>0</v>
-      </c>
-      <c r="J73" s="1">
+      <c r="H73" s="4">
+        <v>0</v>
+      </c>
+      <c r="I73" s="4">
+        <v>0</v>
+      </c>
+      <c r="J73" s="4">
         <v>0</v>
       </c>
       <c r="K73" t="s">
@@ -7081,22 +7105,22 @@
       <c r="D74" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="4">
         <v>0.05</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="4">
         <v>0.1</v>
       </c>
-      <c r="G74" s="1">
+      <c r="G74" s="4">
         <v>0.15</v>
       </c>
-      <c r="H74" s="1">
-        <v>0</v>
-      </c>
-      <c r="I74" s="1">
-        <v>0</v>
-      </c>
-      <c r="J74" s="1">
+      <c r="H74" s="4">
+        <v>0</v>
+      </c>
+      <c r="I74" s="4">
+        <v>0</v>
+      </c>
+      <c r="J74" s="4">
         <v>0</v>
       </c>
       <c r="K74" t="s">
@@ -7167,22 +7191,22 @@
       <c r="D75" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75" s="4">
         <v>0.25</v>
       </c>
-      <c r="G75" s="1">
-        <v>0</v>
-      </c>
-      <c r="H75" s="1">
+      <c r="G75" s="4">
+        <v>0</v>
+      </c>
+      <c r="H75" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I75" s="1">
-        <v>0</v>
-      </c>
-      <c r="J75" s="1">
+      <c r="I75" s="4">
+        <v>0</v>
+      </c>
+      <c r="J75" s="4">
         <v>0</v>
       </c>
       <c r="K75" t="s">
@@ -7250,22 +7274,22 @@
       <c r="D76" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="4">
         <v>0.1125</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76" s="4">
         <v>0.125</v>
       </c>
-      <c r="G76" s="1">
+      <c r="G76" s="4">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="H76" s="1">
-        <v>0</v>
-      </c>
-      <c r="I76" s="1">
-        <v>0</v>
-      </c>
-      <c r="J76" s="1">
+      <c r="H76" s="4">
+        <v>0</v>
+      </c>
+      <c r="I76" s="4">
+        <v>0</v>
+      </c>
+      <c r="J76" s="4">
         <v>0</v>
       </c>
       <c r="K76" t="s">
@@ -7336,22 +7360,22 @@
       <c r="D77" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77" s="4">
         <v>0.25</v>
       </c>
-      <c r="G77" s="1">
-        <v>0</v>
-      </c>
-      <c r="H77" s="1">
+      <c r="G77" s="4">
+        <v>0</v>
+      </c>
+      <c r="H77" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I77" s="1">
-        <v>0</v>
-      </c>
-      <c r="J77" s="1">
+      <c r="I77" s="4">
+        <v>0</v>
+      </c>
+      <c r="J77" s="4">
         <v>0</v>
       </c>
       <c r="K77" t="s">
@@ -7422,22 +7446,22 @@
       <c r="D78" t="s">
         <v>12</v>
       </c>
-      <c r="E78" s="1">
-        <v>0</v>
-      </c>
-      <c r="F78" s="1">
+      <c r="E78" s="4">
+        <v>0</v>
+      </c>
+      <c r="F78" s="4">
         <v>0.05</v>
       </c>
-      <c r="G78" s="1">
+      <c r="G78" s="4">
         <v>0.3</v>
       </c>
-      <c r="H78" s="1">
-        <v>0</v>
-      </c>
-      <c r="I78" s="1">
-        <v>0</v>
-      </c>
-      <c r="J78" s="1">
+      <c r="H78" s="4">
+        <v>0</v>
+      </c>
+      <c r="I78" s="4">
+        <v>0</v>
+      </c>
+      <c r="J78" s="4">
         <v>0</v>
       </c>
       <c r="K78" t="s">
@@ -7508,22 +7532,22 @@
       <c r="D79" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="1">
-        <v>0</v>
-      </c>
-      <c r="F79" s="1">
+      <c r="E79" s="4">
+        <v>0</v>
+      </c>
+      <c r="F79" s="4">
         <v>0.05</v>
       </c>
-      <c r="G79" s="1">
+      <c r="G79" s="4">
         <v>0.3</v>
       </c>
-      <c r="H79" s="1">
-        <v>0</v>
-      </c>
-      <c r="I79" s="1">
-        <v>0</v>
-      </c>
-      <c r="J79" s="1">
+      <c r="H79" s="4">
+        <v>0</v>
+      </c>
+      <c r="I79" s="4">
+        <v>0</v>
+      </c>
+      <c r="J79" s="4">
         <v>0</v>
       </c>
       <c r="K79" t="s">
@@ -7594,22 +7618,22 @@
       <c r="D80" t="s">
         <v>12</v>
       </c>
-      <c r="E80" s="1">
-        <v>0</v>
-      </c>
-      <c r="F80" s="1">
+      <c r="E80" s="4">
+        <v>0</v>
+      </c>
+      <c r="F80" s="4">
         <v>0.05</v>
       </c>
-      <c r="G80" s="1">
+      <c r="G80" s="4">
         <v>0.3</v>
       </c>
-      <c r="H80" s="1">
-        <v>0</v>
-      </c>
-      <c r="I80" s="1">
-        <v>0</v>
-      </c>
-      <c r="J80" s="1">
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="4">
+        <v>0</v>
+      </c>
+      <c r="J80" s="4">
         <v>0</v>
       </c>
       <c r="K80" t="s">
@@ -7680,22 +7704,22 @@
       <c r="D81" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="1">
-        <v>0</v>
-      </c>
-      <c r="F81" s="1">
+      <c r="E81" s="4">
+        <v>0</v>
+      </c>
+      <c r="F81" s="4">
         <v>0.05</v>
       </c>
-      <c r="G81" s="1">
+      <c r="G81" s="4">
         <v>0.3</v>
       </c>
-      <c r="H81" s="1">
-        <v>0</v>
-      </c>
-      <c r="I81" s="1">
-        <v>0</v>
-      </c>
-      <c r="J81" s="1">
+      <c r="H81" s="4">
+        <v>0</v>
+      </c>
+      <c r="I81" s="4">
+        <v>0</v>
+      </c>
+      <c r="J81" s="4">
         <v>0</v>
       </c>
       <c r="K81" t="s">
@@ -7766,22 +7790,22 @@
       <c r="D82" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82" s="4">
         <v>0.25</v>
       </c>
-      <c r="G82" s="1">
-        <v>0</v>
-      </c>
-      <c r="H82" s="1">
+      <c r="G82" s="4">
+        <v>0</v>
+      </c>
+      <c r="H82" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I82" s="1">
-        <v>0</v>
-      </c>
-      <c r="J82" s="1">
+      <c r="I82" s="4">
+        <v>0</v>
+      </c>
+      <c r="J82" s="4">
         <v>0</v>
       </c>
       <c r="K82" t="s">
@@ -7849,22 +7873,22 @@
       <c r="D83" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="1">
-        <v>0</v>
-      </c>
-      <c r="F83" s="1">
+      <c r="E83" s="4">
+        <v>0</v>
+      </c>
+      <c r="F83" s="4">
         <v>0.05</v>
       </c>
-      <c r="G83" s="1">
+      <c r="G83" s="4">
         <v>0.3</v>
       </c>
-      <c r="H83" s="1">
-        <v>0</v>
-      </c>
-      <c r="I83" s="1">
-        <v>0</v>
-      </c>
-      <c r="J83" s="1">
+      <c r="H83" s="4">
+        <v>0</v>
+      </c>
+      <c r="I83" s="4">
+        <v>0</v>
+      </c>
+      <c r="J83" s="4">
         <v>0</v>
       </c>
       <c r="K83" t="s">
@@ -7935,22 +7959,22 @@
       <c r="D84" t="s">
         <v>12</v>
       </c>
-      <c r="E84" s="1">
-        <v>0</v>
-      </c>
-      <c r="F84" s="1">
+      <c r="E84" s="4">
+        <v>0</v>
+      </c>
+      <c r="F84" s="4">
         <v>0.05</v>
       </c>
-      <c r="G84" s="1">
+      <c r="G84" s="4">
         <v>0.3</v>
       </c>
-      <c r="H84" s="1">
-        <v>0</v>
-      </c>
-      <c r="I84" s="1">
-        <v>0</v>
-      </c>
-      <c r="J84" s="1">
+      <c r="H84" s="4">
+        <v>0</v>
+      </c>
+      <c r="I84" s="4">
+        <v>0</v>
+      </c>
+      <c r="J84" s="4">
         <v>0</v>
       </c>
       <c r="K84" t="s">
@@ -8021,22 +8045,22 @@
       <c r="D85" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85" s="4">
         <v>0.25</v>
       </c>
-      <c r="G85" s="1">
-        <v>0</v>
-      </c>
-      <c r="H85" s="1">
+      <c r="G85" s="4">
+        <v>0</v>
+      </c>
+      <c r="H85" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I85" s="1">
-        <v>0</v>
-      </c>
-      <c r="J85" s="1">
+      <c r="I85" s="4">
+        <v>0</v>
+      </c>
+      <c r="J85" s="4">
         <v>0</v>
       </c>
       <c r="K85" t="s">

</xml_diff>